<commit_message>
chore: Update Budget Dashboard spreadsheet with latest financial data
</commit_message>
<xml_diff>
--- a/Budget Dashboard/Budget Dashboard.xlsx
+++ b/Budget Dashboard/Budget Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikherring/HigueraAzureFunction/Budget Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B83AA8C1-AF24-4D48-8FF8-4006765016C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D912C65-F7B6-044F-A1C3-7966F393E16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="640" windowWidth="33720" windowHeight="19380" xr2:uid="{9381A355-5750-421D-8844-C63C039EC95F}"/>
+    <workbookView xWindow="3220" yWindow="500" windowWidth="33720" windowHeight="19380" xr2:uid="{9381A355-5750-421D-8844-C63C039EC95F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14536,7 +14536,7 @@
   <dimension ref="A1:V95"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>